<commit_message>
Arreglos diseño, ya no reenvia formulario, fin importar persona
</commit_message>
<xml_diff>
--- a/arc/arc_Libro1.xlsx
+++ b/arc/arc_Libro1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duvanrivera\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA50C4F8-A78E-4FE5-A50B-99B5B8CA2C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94B5CC9-25A5-4CA8-B4B1-2CBED4FDAA81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10185" yWindow="2025" windowWidth="19650" windowHeight="11385" xr2:uid="{AC666F3B-5823-41FB-96A7-40BA11624A31}"/>
+    <workbookView xWindow="255" yWindow="1695" windowWidth="18180" windowHeight="11385" xr2:uid="{AC666F3B-5823-41FB-96A7-40BA11624A31}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -187,10 +187,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -213,13 +221,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -535,7 +546,7 @@
   <dimension ref="B3:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,6 +571,7 @@
       <c r="E3">
         <v>1069304404</v>
       </c>
+      <c r="F3" s="1"/>
       <c r="G3" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Importar equipos casi terminado
</commit_message>
<xml_diff>
--- a/arc/arc_Libro1.xlsx
+++ b/arc/arc_Libro1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duvanrivera\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94B5CC9-25A5-4CA8-B4B1-2CBED4FDAA81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FC6760-CA52-488F-B06A-4CF2F542E0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="255" yWindow="1695" windowWidth="18180" windowHeight="11385" xr2:uid="{AC666F3B-5823-41FB-96A7-40BA11624A31}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>APRENDIZ SENA</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>JULIAN DAVID</t>
+  </si>
+  <si>
+    <t>rrhh@galqui.com</t>
   </si>
 </sst>
 </file>
@@ -543,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78ABAF4D-8D4E-4C34-82E1-BB8F60C584FB}">
-  <dimension ref="B3:I13"/>
+  <dimension ref="B3:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +561,7 @@
     <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>41</v>
       </c>
@@ -571,7 +574,9 @@
       <c r="E3">
         <v>1069304404</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="G3" t="s">
         <v>0</v>
       </c>
@@ -581,8 +586,11 @@
       <c r="I3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>42</v>
       </c>
@@ -607,8 +615,11 @@
       <c r="I4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>43</v>
       </c>
@@ -633,8 +644,11 @@
       <c r="I5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>44</v>
       </c>
@@ -659,8 +673,11 @@
       <c r="I6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>45</v>
       </c>
@@ -680,10 +697,13 @@
         <v>20</v>
       </c>
       <c r="I7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>46</v>
       </c>
@@ -708,8 +728,11 @@
       <c r="I8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>47</v>
       </c>
@@ -732,10 +755,13 @@
         <v>25</v>
       </c>
       <c r="I9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>48</v>
       </c>
@@ -760,8 +786,11 @@
       <c r="I10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>49</v>
       </c>
@@ -784,10 +813,13 @@
         <v>27</v>
       </c>
       <c r="I11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>50</v>
       </c>
@@ -812,8 +844,11 @@
       <c r="I12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>51</v>
       </c>
@@ -838,8 +873,14 @@
       <c r="I13">
         <v>1</v>
       </c>
+      <c r="J13">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{75CF4AAB-01DA-4385-B08B-7135D35D2DB2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Muchas correcciones y casi terminado importar tarjdetas asignadas
</commit_message>
<xml_diff>
--- a/arc/arc_Libro1.xlsx
+++ b/arc/arc_Libro1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duvanrivera\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FC6760-CA52-488F-B06A-4CF2F542E0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0A6EC1-86E0-437E-81B7-33DD8565FCC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="255" yWindow="1695" windowWidth="18180" windowHeight="11385" xr2:uid="{AC666F3B-5823-41FB-96A7-40BA11624A31}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AC666F3B-5823-41FB-96A7-40BA11624A31}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Arreglos importacion tarjetas, control de errores
</commit_message>
<xml_diff>
--- a/arc/arc_Libro1.xlsx
+++ b/arc/arc_Libro1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duvanrivera\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0A6EC1-86E0-437E-81B7-33DD8565FCC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A985FC-ACD8-4BBF-9C09-70D190F5BB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AC666F3B-5823-41FB-96A7-40BA11624A31}"/>
+    <workbookView xWindow="870" yWindow="2400" windowWidth="13350" windowHeight="11385" xr2:uid="{AC666F3B-5823-41FB-96A7-40BA11624A31}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -207,12 +207,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -228,9 +234,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -549,7 +556,7 @@
   <dimension ref="B3:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:J13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +578,7 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>1069304404</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -600,7 +607,7 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>80200165</v>
       </c>
       <c r="F4" t="s">
@@ -629,7 +636,7 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>1055314236</v>
       </c>
       <c r="F5" t="s">
@@ -658,7 +665,7 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>1024530115</v>
       </c>
       <c r="F6" t="s">
@@ -687,7 +694,7 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>1076240985</v>
       </c>
       <c r="G7" t="s">
@@ -713,7 +720,7 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>80370195</v>
       </c>
       <c r="F8" t="s">
@@ -771,7 +778,7 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>1100953829</v>
       </c>
       <c r="F10" t="s">
@@ -800,7 +807,7 @@
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>80059515</v>
       </c>
       <c r="F11" t="s">

</xml_diff>

<commit_message>
Finalizacion funciones de importacion
</commit_message>
<xml_diff>
--- a/arc/arc_Libro1.xlsx
+++ b/arc/arc_Libro1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duvanrivera\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A985FC-ACD8-4BBF-9C09-70D190F5BB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2161C97B-2BE3-4230-8BA3-4C87DEDE2799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="2400" windowWidth="13350" windowHeight="11385" xr2:uid="{AC666F3B-5823-41FB-96A7-40BA11624A31}"/>
+    <workbookView xWindow="1530" yWindow="3030" windowWidth="13350" windowHeight="11385" xr2:uid="{AC666F3B-5823-41FB-96A7-40BA11624A31}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -556,7 +556,7 @@
   <dimension ref="B3:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>